<commit_message>
13 clusters: code and results
</commit_message>
<xml_diff>
--- a/project/Res-Analysis/MoreThan2Clusters.xlsx
+++ b/project/Res-Analysis/MoreThan2Clusters.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="0" windowWidth="27720" windowHeight="17340" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1000" yWindow="0" windowWidth="27720" windowHeight="17340" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="10 Clusters" sheetId="1" r:id="rId1"/>
-    <sheet name="5 Clusters" sheetId="2" r:id="rId2"/>
-    <sheet name="3 Clusters" sheetId="3" r:id="rId3"/>
+    <sheet name="13 Clusters" sheetId="4" r:id="rId1"/>
+    <sheet name="10 Clusters" sheetId="1" r:id="rId2"/>
+    <sheet name="5 Clusters" sheetId="2" r:id="rId3"/>
+    <sheet name="3 Clusters" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="28">
   <si>
     <t>L9</t>
   </si>
@@ -96,6 +97,15 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>L10</t>
+  </si>
+  <si>
+    <t>L11</t>
+  </si>
+  <si>
+    <t>L12</t>
   </si>
 </sst>
 </file>
@@ -249,8 +259,66 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="135">
+  <cellStyleXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -405,7 +473,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="135">
+  <cellStyles count="193">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -473,6 +541,35 @@
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -540,6 +637,35 @@
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -869,15 +995,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" customWidth="1"/>
+    <col min="13" max="13" width="8.5" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" customWidth="1"/>
+    <col min="15" max="15" width="8.6640625" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" customWidth="1"/>
+    <col min="17" max="17" width="8.33203125" customWidth="1"/>
+    <col min="18" max="18" width="5.6640625" customWidth="1"/>
+    <col min="19" max="19" width="9.33203125" customWidth="1"/>
+    <col min="20" max="20" width="7.83203125" customWidth="1"/>
+    <col min="21" max="21" width="8.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -961,185 +1104,185 @@
       </c>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="8">
-        <v>11</v>
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>0.12</v>
+        <v>0.33</v>
       </c>
       <c r="D3">
+        <v>0.17</v>
+      </c>
+      <c r="E3">
+        <v>0.22</v>
+      </c>
+      <c r="G3">
+        <v>0.67</v>
+      </c>
+      <c r="H3">
+        <v>0.33</v>
+      </c>
+      <c r="I3">
+        <v>0.44</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="O3">
         <v>0.27</v>
       </c>
-      <c r="E3">
-        <v>0.16</v>
-      </c>
-      <c r="G3">
+      <c r="P3">
+        <v>0.5</v>
+      </c>
+      <c r="Q3">
+        <v>0.35</v>
+      </c>
+      <c r="S3">
+        <v>0.75</v>
+      </c>
+      <c r="T3">
+        <v>0.5</v>
+      </c>
+      <c r="U3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0.4</v>
+      </c>
+      <c r="D4">
+        <v>0.67</v>
+      </c>
+      <c r="E4">
+        <v>0.5</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0.67</v>
+      </c>
+      <c r="I4">
         <v>0.8</v>
       </c>
-      <c r="H3">
-        <v>0.36</v>
-      </c>
-      <c r="I3">
-        <v>0.5</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0.12</v>
-      </c>
-      <c r="P3">
-        <v>0.27</v>
-      </c>
-      <c r="Q3">
-        <v>0.17</v>
-      </c>
-      <c r="S3">
-        <v>0.36</v>
-      </c>
-      <c r="T3">
-        <v>0.36</v>
-      </c>
-      <c r="U3">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="8">
-        <v>6</v>
-      </c>
-      <c r="C4">
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0.15</v>
+      </c>
+      <c r="P4">
+        <v>0.67</v>
+      </c>
+      <c r="Q4">
+        <v>0.25</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
         <v>0.38</v>
       </c>
-      <c r="D4">
-        <v>0.5</v>
-      </c>
-      <c r="E4">
-        <v>0.43</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0.5</v>
-      </c>
-      <c r="I4">
-        <v>0.67</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="P4">
-        <v>0.5</v>
-      </c>
-      <c r="Q4">
-        <v>0.22</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4">
-        <v>0.5</v>
-      </c>
-      <c r="U4">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="8">
-        <v>393</v>
-      </c>
-      <c r="C5">
-        <v>0.75</v>
-      </c>
-      <c r="D5">
-        <v>0.69</v>
-      </c>
-      <c r="E5">
-        <v>0.72</v>
-      </c>
-      <c r="G5">
-        <v>0.78</v>
-      </c>
-      <c r="H5">
-        <v>0.95</v>
-      </c>
-      <c r="I5">
-        <v>0.86</v>
-      </c>
-      <c r="K5">
-        <v>0.72</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>0.84</v>
-      </c>
-      <c r="O5">
-        <v>0.84</v>
-      </c>
-      <c r="P5">
-        <v>0.05</v>
-      </c>
-      <c r="Q5">
-        <v>0.1</v>
-      </c>
-      <c r="S5">
-        <v>0.76</v>
-      </c>
-      <c r="T5">
-        <v>0.82</v>
-      </c>
-      <c r="U5">
-        <v>0.79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="A6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="8">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>0.36</v>
-      </c>
       <c r="D6">
-        <v>0.71</v>
+        <v>0.6</v>
       </c>
       <c r="E6">
-        <v>0.48</v>
+        <v>0.46</v>
       </c>
       <c r="G6">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>0.86</v>
+        <v>0.6</v>
       </c>
       <c r="I6">
         <v>0.75</v>
@@ -1154,339 +1297,498 @@
         <v>0</v>
       </c>
       <c r="O6">
+        <v>0.23</v>
+      </c>
+      <c r="P6">
+        <v>0.6</v>
+      </c>
+      <c r="Q6">
+        <v>0.33</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>0.6</v>
+      </c>
+      <c r="U6">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>393</v>
+      </c>
+      <c r="C8">
+        <v>0.77</v>
+      </c>
+      <c r="D8">
+        <v>0.73</v>
+      </c>
+      <c r="E8">
+        <v>0.75</v>
+      </c>
+      <c r="G8">
+        <v>0.78</v>
+      </c>
+      <c r="H8">
+        <v>0.92</v>
+      </c>
+      <c r="I8">
+        <v>0.85</v>
+      </c>
+      <c r="K8">
+        <v>0.72</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>0.84</v>
+      </c>
+      <c r="O8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P8">
+        <v>0.03</v>
+      </c>
+      <c r="Q8">
+        <v>0.06</v>
+      </c>
+      <c r="S8">
+        <v>0.75</v>
+      </c>
+      <c r="T8">
+        <v>0.82</v>
+      </c>
+      <c r="U8">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>0.46</v>
+      </c>
+      <c r="D9">
+        <v>0.86</v>
+      </c>
+      <c r="E9">
+        <v>0.6</v>
+      </c>
+      <c r="G9">
+        <v>0.67</v>
+      </c>
+      <c r="H9">
+        <v>0.86</v>
+      </c>
+      <c r="I9">
+        <v>0.75</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0.15</v>
+      </c>
+      <c r="P9">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="Q9">
         <v>0.2</v>
       </c>
-      <c r="P6">
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>106</v>
+      </c>
+      <c r="C10">
+        <v>0.23</v>
+      </c>
+      <c r="D10">
+        <v>0.2</v>
+      </c>
+      <c r="E10">
+        <v>0.21</v>
+      </c>
+      <c r="G10">
+        <v>0.43</v>
+      </c>
+      <c r="H10">
+        <v>0.22</v>
+      </c>
+      <c r="I10">
         <v>0.28999999999999998</v>
       </c>
-      <c r="Q6">
-        <v>0.24</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
-      <c r="A7" s="6" t="s">
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0.19</v>
+      </c>
+      <c r="P10">
+        <v>0.42</v>
+      </c>
+      <c r="Q10">
+        <v>0.26</v>
+      </c>
+      <c r="S10">
+        <v>0.35</v>
+      </c>
+      <c r="T10">
+        <v>0.34</v>
+      </c>
+      <c r="U10">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D11">
+        <v>0.67</v>
+      </c>
+      <c r="E11">
+        <v>0.62</v>
+      </c>
+      <c r="G11">
+        <v>0.75</v>
+      </c>
+      <c r="H11">
+        <v>0.5</v>
+      </c>
+      <c r="I11">
+        <v>0.6</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0.33</v>
+      </c>
+      <c r="M11">
+        <v>0.5</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>0.75</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0.86</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>0.67</v>
+      </c>
+      <c r="Q12">
+        <v>0.8</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>0.33</v>
+      </c>
+      <c r="D13">
+        <v>0.43</v>
+      </c>
+      <c r="E13">
+        <v>0.38</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0.43</v>
+      </c>
+      <c r="I13">
+        <v>0.6</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0.06</v>
+      </c>
+      <c r="P13">
+        <v>0.86</v>
+      </c>
+      <c r="Q13">
+        <v>0.1</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
         <v>4</v>
       </c>
-      <c r="B7" s="8">
-        <v>106</v>
-      </c>
-      <c r="C7">
-        <v>0.23</v>
-      </c>
-      <c r="D7">
-        <v>0.23</v>
-      </c>
-      <c r="E7">
-        <v>0.23</v>
-      </c>
-      <c r="G7">
-        <v>0.52</v>
-      </c>
-      <c r="H7">
-        <v>0.21</v>
-      </c>
-      <c r="I7">
-        <v>0.3</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0.2</v>
-      </c>
-      <c r="P7">
+      <c r="C14">
+        <v>0.5</v>
+      </c>
+      <c r="D14">
+        <v>0.75</v>
+      </c>
+      <c r="E14">
+        <v>0.6</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0.5</v>
+      </c>
+      <c r="I14">
+        <v>0.67</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0.03</v>
+      </c>
+      <c r="P14">
+        <v>0.75</v>
+      </c>
+      <c r="Q14">
+        <v>0.06</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>0.31</v>
+      </c>
+      <c r="D15">
+        <v>0.83</v>
+      </c>
+      <c r="E15">
         <v>0.45</v>
       </c>
-      <c r="Q7">
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0.83</v>
+      </c>
+      <c r="I15">
+        <v>0.91</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>0.5</v>
+      </c>
+      <c r="M15">
+        <v>0.67</v>
+      </c>
+      <c r="O15">
         <v>0.27</v>
       </c>
-      <c r="S7">
-        <v>0.36</v>
-      </c>
-      <c r="T7">
-        <v>0.34</v>
-      </c>
-      <c r="U7">
+      <c r="P15">
+        <v>0.5</v>
+      </c>
+      <c r="Q15">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="8" spans="1:21">
-      <c r="A8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="8">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>0.44</v>
-      </c>
-      <c r="D8">
-        <v>0.67</v>
-      </c>
-      <c r="E8">
-        <v>0.53</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>0.5</v>
-      </c>
-      <c r="I8">
-        <v>0.67</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <v>0.33</v>
-      </c>
-      <c r="M8">
-        <v>0.5</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="A9" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="8">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>0.67</v>
-      </c>
-      <c r="D9">
-        <v>0.67</v>
-      </c>
-      <c r="E9">
-        <v>0.67</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="P9">
-        <v>0.67</v>
-      </c>
-      <c r="Q9">
-        <v>0.8</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
-      <c r="A10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="8">
-        <v>7</v>
-      </c>
-      <c r="C10">
-        <v>0.5</v>
-      </c>
-      <c r="D10">
-        <v>0.43</v>
-      </c>
-      <c r="E10">
-        <v>0.46</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="I10">
-        <v>0.44</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0.06</v>
-      </c>
-      <c r="P10">
-        <v>0.86</v>
-      </c>
-      <c r="Q10">
-        <v>0.11</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
-      <c r="A11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="8">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>0.5</v>
-      </c>
-      <c r="D11">
-        <v>0.75</v>
-      </c>
-      <c r="E11">
-        <v>0.6</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>0.75</v>
-      </c>
-      <c r="I11">
-        <v>0.86</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0.12</v>
-      </c>
-      <c r="P11">
-        <v>0.75</v>
-      </c>
-      <c r="Q11">
-        <v>0.21</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
-      <c r="A12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="8">
-        <v>6</v>
-      </c>
-      <c r="C12">
-        <v>0.42</v>
-      </c>
-      <c r="D12">
-        <v>0.83</v>
-      </c>
-      <c r="E12">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>0.83</v>
-      </c>
-      <c r="I12">
-        <v>0.91</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>0.5</v>
-      </c>
-      <c r="M12">
-        <v>0.67</v>
-      </c>
-      <c r="O12">
-        <v>0.18</v>
-      </c>
-      <c r="P12">
-        <v>0.5</v>
-      </c>
-      <c r="Q12">
-        <v>0.26</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12">
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
         <v>0</v>
       </c>
     </row>
@@ -1502,6 +1804,640 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:U2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="3"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="4"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="5"/>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="8">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>0.12</v>
+      </c>
+      <c r="D3">
+        <v>0.27</v>
+      </c>
+      <c r="E3">
+        <v>0.16</v>
+      </c>
+      <c r="G3">
+        <v>0.8</v>
+      </c>
+      <c r="H3">
+        <v>0.36</v>
+      </c>
+      <c r="I3">
+        <v>0.5</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0.12</v>
+      </c>
+      <c r="P3">
+        <v>0.27</v>
+      </c>
+      <c r="Q3">
+        <v>0.17</v>
+      </c>
+      <c r="S3">
+        <v>0.36</v>
+      </c>
+      <c r="T3">
+        <v>0.36</v>
+      </c>
+      <c r="U3">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>0.38</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+      <c r="E4">
+        <v>0.43</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0.5</v>
+      </c>
+      <c r="I4">
+        <v>0.67</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="P4">
+        <v>0.5</v>
+      </c>
+      <c r="Q4">
+        <v>0.22</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>0.5</v>
+      </c>
+      <c r="U4">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8">
+        <v>393</v>
+      </c>
+      <c r="C5">
+        <v>0.75</v>
+      </c>
+      <c r="D5">
+        <v>0.69</v>
+      </c>
+      <c r="E5">
+        <v>0.72</v>
+      </c>
+      <c r="G5">
+        <v>0.78</v>
+      </c>
+      <c r="H5">
+        <v>0.95</v>
+      </c>
+      <c r="I5">
+        <v>0.86</v>
+      </c>
+      <c r="K5">
+        <v>0.72</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0.84</v>
+      </c>
+      <c r="O5">
+        <v>0.84</v>
+      </c>
+      <c r="P5">
+        <v>0.05</v>
+      </c>
+      <c r="Q5">
+        <v>0.1</v>
+      </c>
+      <c r="S5">
+        <v>0.76</v>
+      </c>
+      <c r="T5">
+        <v>0.82</v>
+      </c>
+      <c r="U5">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="8">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>0.36</v>
+      </c>
+      <c r="D6">
+        <v>0.71</v>
+      </c>
+      <c r="E6">
+        <v>0.48</v>
+      </c>
+      <c r="G6">
+        <v>0.67</v>
+      </c>
+      <c r="H6">
+        <v>0.86</v>
+      </c>
+      <c r="I6">
+        <v>0.75</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0.2</v>
+      </c>
+      <c r="P6">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="Q6">
+        <v>0.24</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="8">
+        <v>106</v>
+      </c>
+      <c r="C7">
+        <v>0.23</v>
+      </c>
+      <c r="D7">
+        <v>0.23</v>
+      </c>
+      <c r="E7">
+        <v>0.23</v>
+      </c>
+      <c r="G7">
+        <v>0.52</v>
+      </c>
+      <c r="H7">
+        <v>0.21</v>
+      </c>
+      <c r="I7">
+        <v>0.3</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0.2</v>
+      </c>
+      <c r="P7">
+        <v>0.45</v>
+      </c>
+      <c r="Q7">
+        <v>0.27</v>
+      </c>
+      <c r="S7">
+        <v>0.36</v>
+      </c>
+      <c r="T7">
+        <v>0.34</v>
+      </c>
+      <c r="U7">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>0.44</v>
+      </c>
+      <c r="D8">
+        <v>0.67</v>
+      </c>
+      <c r="E8">
+        <v>0.53</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0.5</v>
+      </c>
+      <c r="I8">
+        <v>0.67</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0.33</v>
+      </c>
+      <c r="M8">
+        <v>0.5</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>0.67</v>
+      </c>
+      <c r="D9">
+        <v>0.67</v>
+      </c>
+      <c r="E9">
+        <v>0.67</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>0.67</v>
+      </c>
+      <c r="Q9">
+        <v>0.8</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="8">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+      <c r="D10">
+        <v>0.43</v>
+      </c>
+      <c r="E10">
+        <v>0.46</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I10">
+        <v>0.44</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0.06</v>
+      </c>
+      <c r="P10">
+        <v>0.86</v>
+      </c>
+      <c r="Q10">
+        <v>0.11</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="8">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>0.5</v>
+      </c>
+      <c r="D11">
+        <v>0.75</v>
+      </c>
+      <c r="E11">
+        <v>0.6</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0.75</v>
+      </c>
+      <c r="I11">
+        <v>0.86</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0.12</v>
+      </c>
+      <c r="P11">
+        <v>0.75</v>
+      </c>
+      <c r="Q11">
+        <v>0.21</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="8">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>0.42</v>
+      </c>
+      <c r="D12">
+        <v>0.83</v>
+      </c>
+      <c r="E12">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0.83</v>
+      </c>
+      <c r="I12">
+        <v>0.91</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>0.5</v>
+      </c>
+      <c r="M12">
+        <v>0.67</v>
+      </c>
+      <c r="O12">
+        <v>0.18</v>
+      </c>
+      <c r="P12">
+        <v>0.5</v>
+      </c>
+      <c r="Q12">
+        <v>0.26</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U7"/>
   <sheetViews>
@@ -1873,11 +2809,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="S1" sqref="S1:U5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
param testing of rand.forest
</commit_message>
<xml_diff>
--- a/project/Res-Analysis/MoreThan2Clusters.xlsx
+++ b/project/Res-Analysis/MoreThan2Clusters.xlsx
@@ -4,14 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1140" windowWidth="27720" windowHeight="17340" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="13 Clusters" sheetId="4" r:id="rId1"/>
     <sheet name="12 Clusters" sheetId="5" r:id="rId2"/>
-    <sheet name="10 Clusters" sheetId="1" r:id="rId3"/>
-    <sheet name="5 Clusters" sheetId="2" r:id="rId4"/>
-    <sheet name="3 Clusters" sheetId="3" r:id="rId5"/>
+    <sheet name="5 Clusters" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="28">
   <si>
     <t>L9</t>
   </si>
@@ -113,7 +111,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,30 +158,8 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="12">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,36 +196,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEBF1DE"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE4DFEC"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDAEEF3"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFDE9D9"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDD9C4"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -260,7 +206,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="231">
+  <cellStyleXfs count="291">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -492,8 +438,68 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -503,16 +509,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="231">
+  <cellStyles count="291">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -628,6 +626,36 @@
     <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -743,6 +771,36 @@
     <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1075,7 +1133,7 @@
   <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:U2"/>
+      <selection activeCell="B3" sqref="B3:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1181,29 +1239,29 @@
       </c>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="8">
         <v>6</v>
       </c>
       <c r="C3">
-        <v>0.33</v>
+        <v>0.1</v>
       </c>
       <c r="D3">
         <v>0.17</v>
       </c>
       <c r="E3">
-        <v>0.22</v>
+        <v>0.12</v>
       </c>
       <c r="G3">
-        <v>0.67</v>
+        <v>0.75</v>
       </c>
       <c r="H3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I3">
-        <v>0.44</v>
+        <v>0.6</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1215,13 +1273,13 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>0.27</v>
+        <v>0.21</v>
       </c>
       <c r="P3">
         <v>0.5</v>
       </c>
       <c r="Q3">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="S3">
         <v>0.75</v>
@@ -1234,20 +1292,20 @@
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="8">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="D4">
         <v>0.67</v>
       </c>
       <c r="E4">
-        <v>0.5</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1268,13 +1326,13 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>0.15</v>
+        <v>0.5</v>
       </c>
       <c r="P4">
         <v>0.67</v>
       </c>
       <c r="Q4">
-        <v>0.25</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="S4">
         <v>0</v>
@@ -1287,10 +1345,10 @@
       </c>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="8">
         <v>2</v>
       </c>
       <c r="C5">
@@ -1340,29 +1398,29 @@
       </c>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6">
+      <c r="A6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="8">
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.38</v>
+        <v>0.33</v>
       </c>
       <c r="D6">
         <v>0.6</v>
       </c>
       <c r="E6">
-        <v>0.46</v>
+        <v>0.43</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="H6">
         <v>0.6</v>
       </c>
       <c r="I6">
-        <v>0.75</v>
+        <v>0.67</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -1374,13 +1432,13 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>0.23</v>
+        <v>0.38</v>
       </c>
       <c r="P6">
         <v>0.6</v>
       </c>
       <c r="Q6">
-        <v>0.33</v>
+        <v>0.46</v>
       </c>
       <c r="S6">
         <v>1</v>
@@ -1393,10 +1451,10 @@
       </c>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="8">
         <v>1</v>
       </c>
       <c r="C7">
@@ -1446,26 +1504,26 @@
       </c>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" t="s">
+      <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="8">
         <v>393</v>
       </c>
       <c r="C8">
         <v>0.77</v>
       </c>
       <c r="D8">
-        <v>0.73</v>
+        <v>0.7</v>
       </c>
       <c r="E8">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="G8">
-        <v>0.78</v>
+        <v>0.77</v>
       </c>
       <c r="H8">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="I8">
         <v>0.85</v>
@@ -1480,13 +1538,13 @@
         <v>0.84</v>
       </c>
       <c r="O8">
-        <v>0.55000000000000004</v>
+        <v>0.81</v>
       </c>
       <c r="P8">
-        <v>0.03</v>
+        <v>0.11</v>
       </c>
       <c r="Q8">
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
       <c r="S8">
         <v>0.75</v>
@@ -1499,20 +1557,20 @@
       </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" t="s">
+      <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="8">
         <v>7</v>
       </c>
       <c r="C9">
-        <v>0.46</v>
+        <v>0.43</v>
       </c>
       <c r="D9">
         <v>0.86</v>
       </c>
       <c r="E9">
-        <v>0.6</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="G9">
         <v>0.67</v>
@@ -1533,13 +1591,13 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>0.15</v>
+        <v>0.31</v>
       </c>
       <c r="P9">
-        <v>0.28999999999999998</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="Q9">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="S9">
         <v>0</v>
@@ -1552,47 +1610,47 @@
       </c>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" t="s">
+      <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="8">
         <v>106</v>
       </c>
       <c r="C10">
-        <v>0.23</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D10">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="E10">
+        <v>0.26</v>
+      </c>
+      <c r="G10">
+        <v>0.38</v>
+      </c>
+      <c r="H10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I10">
         <v>0.21</v>
       </c>
-      <c r="G10">
-        <v>0.43</v>
-      </c>
-      <c r="H10">
-        <v>0.22</v>
-      </c>
-      <c r="I10">
-        <v>0.28999999999999998</v>
-      </c>
       <c r="K10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="O10">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="P10">
         <v>0.42</v>
       </c>
       <c r="Q10">
-        <v>0.26</v>
+        <v>0.24</v>
       </c>
       <c r="S10">
         <v>0.35</v>
@@ -1605,32 +1663,32 @@
       </c>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" t="s">
+      <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="8">
         <v>6</v>
       </c>
       <c r="C11">
-        <v>0.56999999999999995</v>
+        <v>0.25</v>
       </c>
       <c r="D11">
-        <v>0.67</v>
+        <v>0.5</v>
       </c>
       <c r="E11">
-        <v>0.62</v>
+        <v>0.33</v>
       </c>
       <c r="G11">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <v>0.5</v>
       </c>
       <c r="I11">
-        <v>0.6</v>
+        <v>0.67</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11">
         <v>0.33</v>
@@ -1639,13 +1697,13 @@
         <v>0.5</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="S11">
         <v>0</v>
@@ -1658,20 +1716,20 @@
       </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" t="s">
+      <c r="A12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="8">
         <v>3</v>
       </c>
       <c r="C12">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12">
-        <v>0.86</v>
+        <v>0.67</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1711,17 +1769,17 @@
       </c>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" t="s">
+      <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="8">
         <v>7</v>
       </c>
       <c r="C13">
-        <v>0.33</v>
+        <v>0.26</v>
       </c>
       <c r="D13">
-        <v>0.43</v>
+        <v>0.71</v>
       </c>
       <c r="E13">
         <v>0.38</v>
@@ -1730,13 +1788,13 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>0.43</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="I13">
-        <v>0.6</v>
+        <v>0.44</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -1751,7 +1809,7 @@
         <v>0.86</v>
       </c>
       <c r="Q13">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="S13">
         <v>0</v>
@@ -1764,29 +1822,29 @@
       </c>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" t="s">
+      <c r="A14" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="8">
         <v>4</v>
       </c>
       <c r="C14">
-        <v>0.5</v>
+        <v>0.38</v>
       </c>
       <c r="D14">
         <v>0.75</v>
       </c>
       <c r="E14">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="I14">
-        <v>0.67</v>
+        <v>0.86</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1798,13 +1856,13 @@
         <v>0</v>
       </c>
       <c r="O14">
-        <v>0.03</v>
+        <v>0.3</v>
       </c>
       <c r="P14">
         <v>0.75</v>
       </c>
       <c r="Q14">
-        <v>0.06</v>
+        <v>0.43</v>
       </c>
       <c r="S14">
         <v>0</v>
@@ -1817,20 +1875,20 @@
       </c>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" t="s">
+      <c r="A15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="8">
         <v>6</v>
       </c>
       <c r="C15">
-        <v>0.31</v>
+        <v>0.83</v>
       </c>
       <c r="D15">
         <v>0.83</v>
       </c>
       <c r="E15">
-        <v>0.45</v>
+        <v>0.83</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1884,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:U14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1992,29 +2050,29 @@
       </c>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="8">
         <v>6</v>
       </c>
       <c r="C3">
-        <v>0.33</v>
+        <v>0.27</v>
       </c>
       <c r="D3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E3">
-        <v>0.33</v>
+        <v>0.35</v>
       </c>
       <c r="G3">
-        <v>0.67</v>
+        <v>0.5</v>
       </c>
       <c r="H3">
-        <v>0.33</v>
+        <v>0.17</v>
       </c>
       <c r="I3">
-        <v>0.44</v>
+        <v>0.25</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2026,13 +2084,13 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>0.33</v>
+        <v>0.21</v>
       </c>
       <c r="P3">
         <v>0.5</v>
       </c>
       <c r="Q3">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="S3">
         <v>0</v>
@@ -2045,29 +2103,29 @@
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="8">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D4">
         <v>0.67</v>
       </c>
       <c r="E4">
-        <v>0.5</v>
+        <v>0.44</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0.67</v>
       </c>
       <c r="H4">
         <v>0.67</v>
       </c>
       <c r="I4">
-        <v>0.8</v>
+        <v>0.67</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -2079,13 +2137,13 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>0.14000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="P4">
         <v>0.67</v>
       </c>
       <c r="Q4">
-        <v>0.24</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="S4">
         <v>0</v>
@@ -2098,10 +2156,10 @@
       </c>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="8">
         <v>2</v>
       </c>
       <c r="C5">
@@ -2151,10 +2209,10 @@
       </c>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6">
+      <c r="A6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8">
         <v>6</v>
       </c>
       <c r="C6">
@@ -2185,13 +2243,13 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>0.13</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="P6">
         <v>0.5</v>
       </c>
       <c r="Q6">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="S6">
         <v>0.5</v>
@@ -2204,29 +2262,29 @@
       </c>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="8">
         <v>393</v>
       </c>
       <c r="C7">
         <v>0.77</v>
       </c>
       <c r="D7">
-        <v>0.71</v>
+        <v>0.72</v>
       </c>
       <c r="E7">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
       <c r="G7">
         <v>0.77</v>
       </c>
       <c r="H7">
-        <v>0.91</v>
+        <v>0.94</v>
       </c>
       <c r="I7">
-        <v>0.84</v>
+        <v>0.85</v>
       </c>
       <c r="K7">
         <v>0.72</v>
@@ -2238,13 +2296,13 @@
         <v>0.84</v>
       </c>
       <c r="O7">
-        <v>0.6</v>
+        <v>0.81</v>
       </c>
       <c r="P7">
-        <v>0.03</v>
+        <v>0.11</v>
       </c>
       <c r="Q7">
-        <v>0.06</v>
+        <v>0.19</v>
       </c>
       <c r="S7">
         <v>0.75</v>
@@ -2257,20 +2315,20 @@
       </c>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" t="s">
+      <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="8">
         <v>7</v>
       </c>
       <c r="C8">
-        <v>0.67</v>
+        <v>0.38</v>
       </c>
       <c r="D8">
         <v>0.86</v>
       </c>
       <c r="E8">
-        <v>0.75</v>
+        <v>0.52</v>
       </c>
       <c r="G8">
         <v>0.67</v>
@@ -2291,66 +2349,66 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>0.09</v>
+        <v>0.25</v>
       </c>
       <c r="P8">
+        <v>0.43</v>
+      </c>
+      <c r="Q8">
+        <v>0.32</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="8">
+        <v>106</v>
+      </c>
+      <c r="C9">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D9">
+        <v>0.26</v>
+      </c>
+      <c r="E9">
+        <v>0.27</v>
+      </c>
+      <c r="G9">
+        <v>0.43</v>
+      </c>
+      <c r="H9">
         <v>0.14000000000000001</v>
       </c>
-      <c r="Q8">
-        <v>0.11</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>106</v>
-      </c>
-      <c r="C9">
-        <v>0.19</v>
-      </c>
-      <c r="D9">
-        <v>0.19</v>
-      </c>
-      <c r="E9">
-        <v>0.19</v>
-      </c>
-      <c r="G9">
+      <c r="I9">
+        <v>0.21</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>0.01</v>
+      </c>
+      <c r="M9">
+        <v>0.02</v>
+      </c>
+      <c r="O9">
+        <v>0.16</v>
+      </c>
+      <c r="P9">
         <v>0.39</v>
       </c>
-      <c r="H9">
-        <v>0.19</v>
-      </c>
-      <c r="I9">
-        <v>0.25</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0.2</v>
-      </c>
-      <c r="P9">
-        <v>0.42</v>
-      </c>
       <c r="Q9">
-        <v>0.27</v>
+        <v>0.23</v>
       </c>
       <c r="S9">
         <v>0.36</v>
@@ -2363,20 +2421,20 @@
       </c>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" t="s">
+      <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="8">
         <v>6</v>
       </c>
       <c r="C10">
+        <v>0.6</v>
+      </c>
+      <c r="D10">
         <v>0.5</v>
       </c>
-      <c r="D10">
-        <v>0.67</v>
-      </c>
       <c r="E10">
-        <v>0.56999999999999995</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G10">
         <v>0.6</v>
@@ -2397,13 +2455,13 @@
         <v>0.5</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="S10">
         <v>0</v>
@@ -2416,20 +2474,20 @@
       </c>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" t="s">
+      <c r="A11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="8">
         <v>3</v>
       </c>
       <c r="C11">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
-        <v>0.86</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -2469,20 +2527,20 @@
       </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" t="s">
+      <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="8">
         <v>7</v>
       </c>
       <c r="C12">
-        <v>0.33</v>
+        <v>0.22</v>
       </c>
       <c r="D12">
-        <v>0.43</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="E12">
-        <v>0.38</v>
+        <v>0.32</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -2509,7 +2567,7 @@
         <v>0.86</v>
       </c>
       <c r="Q12">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="S12">
         <v>0</v>
@@ -2522,29 +2580,29 @@
       </c>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" t="s">
+      <c r="A13" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="8">
         <v>4</v>
       </c>
       <c r="C13">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="D13">
         <v>0.75</v>
       </c>
       <c r="E13">
-        <v>0.67</v>
+        <v>0.43</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="I13">
-        <v>0.67</v>
+        <v>0.86</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -2556,13 +2614,13 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>0.03</v>
+        <v>0.3</v>
       </c>
       <c r="P13">
         <v>0.75</v>
       </c>
       <c r="Q13">
-        <v>0.06</v>
+        <v>0.43</v>
       </c>
       <c r="S13">
         <v>0</v>
@@ -2575,20 +2633,20 @@
       </c>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" t="s">
+      <c r="A14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="8">
         <v>6</v>
       </c>
       <c r="C14">
-        <v>0.24</v>
+        <v>0.5</v>
       </c>
       <c r="D14">
         <v>0.83</v>
       </c>
       <c r="E14">
-        <v>0.37</v>
+        <v>0.62</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -2609,13 +2667,13 @@
         <v>0.67</v>
       </c>
       <c r="O14">
-        <v>0.27</v>
+        <v>0.33</v>
       </c>
       <c r="P14">
         <v>0.5</v>
       </c>
       <c r="Q14">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="S14">
         <v>0</v>
@@ -2640,15 +2698,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:U2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="12" max="12" width="7.1640625" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="5.6640625" customWidth="1"/>
+    <col min="15" max="15" width="8.83203125" customWidth="1"/>
+    <col min="16" max="16" width="6.83203125" customWidth="1"/>
+    <col min="17" max="17" width="8.33203125" customWidth="1"/>
+    <col min="19" max="19" width="8.83203125" customWidth="1"/>
+    <col min="20" max="20" width="7.5" customWidth="1"/>
+    <col min="21" max="21" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -2733,662 +2809,25 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="6" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B3" s="8">
-        <v>11</v>
+        <v>417</v>
       </c>
       <c r="C3">
-        <v>0.12</v>
+        <v>0.8</v>
       </c>
       <c r="D3">
-        <v>0.27</v>
+        <v>0.78</v>
       </c>
       <c r="E3">
-        <v>0.16</v>
+        <v>0.79</v>
       </c>
       <c r="G3">
         <v>0.8</v>
       </c>
       <c r="H3">
-        <v>0.36</v>
-      </c>
-      <c r="I3">
-        <v>0.5</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0.12</v>
-      </c>
-      <c r="P3">
-        <v>0.27</v>
-      </c>
-      <c r="Q3">
-        <v>0.17</v>
-      </c>
-      <c r="S3">
-        <v>0.36</v>
-      </c>
-      <c r="T3">
-        <v>0.36</v>
-      </c>
-      <c r="U3">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="8">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>0.38</v>
-      </c>
-      <c r="D4">
-        <v>0.5</v>
-      </c>
-      <c r="E4">
-        <v>0.43</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0.5</v>
-      </c>
-      <c r="I4">
-        <v>0.67</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="P4">
-        <v>0.5</v>
-      </c>
-      <c r="Q4">
-        <v>0.22</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4">
-        <v>0.5</v>
-      </c>
-      <c r="U4">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="8">
-        <v>393</v>
-      </c>
-      <c r="C5">
-        <v>0.75</v>
-      </c>
-      <c r="D5">
-        <v>0.69</v>
-      </c>
-      <c r="E5">
-        <v>0.72</v>
-      </c>
-      <c r="G5">
-        <v>0.78</v>
-      </c>
-      <c r="H5">
-        <v>0.95</v>
-      </c>
-      <c r="I5">
-        <v>0.86</v>
-      </c>
-      <c r="K5">
-        <v>0.72</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>0.84</v>
-      </c>
-      <c r="O5">
-        <v>0.84</v>
-      </c>
-      <c r="P5">
-        <v>0.05</v>
-      </c>
-      <c r="Q5">
-        <v>0.1</v>
-      </c>
-      <c r="S5">
-        <v>0.76</v>
-      </c>
-      <c r="T5">
-        <v>0.82</v>
-      </c>
-      <c r="U5">
-        <v>0.79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="A6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="8">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>0.36</v>
-      </c>
-      <c r="D6">
-        <v>0.71</v>
-      </c>
-      <c r="E6">
-        <v>0.48</v>
-      </c>
-      <c r="G6">
-        <v>0.67</v>
-      </c>
-      <c r="H6">
-        <v>0.86</v>
-      </c>
-      <c r="I6">
-        <v>0.75</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0.2</v>
-      </c>
-      <c r="P6">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="Q6">
-        <v>0.24</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
-      <c r="A7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="8">
-        <v>106</v>
-      </c>
-      <c r="C7">
-        <v>0.23</v>
-      </c>
-      <c r="D7">
-        <v>0.23</v>
-      </c>
-      <c r="E7">
-        <v>0.23</v>
-      </c>
-      <c r="G7">
-        <v>0.52</v>
-      </c>
-      <c r="H7">
-        <v>0.21</v>
-      </c>
-      <c r="I7">
-        <v>0.3</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0.2</v>
-      </c>
-      <c r="P7">
-        <v>0.45</v>
-      </c>
-      <c r="Q7">
-        <v>0.27</v>
-      </c>
-      <c r="S7">
-        <v>0.36</v>
-      </c>
-      <c r="T7">
-        <v>0.34</v>
-      </c>
-      <c r="U7">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
-      <c r="A8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="8">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>0.44</v>
-      </c>
-      <c r="D8">
-        <v>0.67</v>
-      </c>
-      <c r="E8">
-        <v>0.53</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>0.5</v>
-      </c>
-      <c r="I8">
-        <v>0.67</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <v>0.33</v>
-      </c>
-      <c r="M8">
-        <v>0.5</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="A9" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="8">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>0.67</v>
-      </c>
-      <c r="D9">
-        <v>0.67</v>
-      </c>
-      <c r="E9">
-        <v>0.67</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="P9">
-        <v>0.67</v>
-      </c>
-      <c r="Q9">
-        <v>0.8</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
-      <c r="A10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="8">
-        <v>7</v>
-      </c>
-      <c r="C10">
-        <v>0.5</v>
-      </c>
-      <c r="D10">
-        <v>0.43</v>
-      </c>
-      <c r="E10">
-        <v>0.46</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="I10">
-        <v>0.44</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0.06</v>
-      </c>
-      <c r="P10">
-        <v>0.86</v>
-      </c>
-      <c r="Q10">
-        <v>0.11</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
-      <c r="A11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="8">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>0.5</v>
-      </c>
-      <c r="D11">
-        <v>0.75</v>
-      </c>
-      <c r="E11">
-        <v>0.6</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>0.75</v>
-      </c>
-      <c r="I11">
-        <v>0.86</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0.12</v>
-      </c>
-      <c r="P11">
-        <v>0.75</v>
-      </c>
-      <c r="Q11">
-        <v>0.21</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
-      <c r="A12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="8">
-        <v>6</v>
-      </c>
-      <c r="C12">
-        <v>0.42</v>
-      </c>
-      <c r="D12">
-        <v>0.83</v>
-      </c>
-      <c r="E12">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>0.83</v>
-      </c>
-      <c r="I12">
-        <v>0.91</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>0.5</v>
-      </c>
-      <c r="M12">
-        <v>0.67</v>
-      </c>
-      <c r="O12">
-        <v>0.18</v>
-      </c>
-      <c r="P12">
-        <v>0.5</v>
-      </c>
-      <c r="Q12">
-        <v>0.26</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:U7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" customWidth="1"/>
-    <col min="14" max="14" width="5.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21">
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="2"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="3"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" s="4"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="5"/>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="A3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="8">
-        <v>471</v>
-      </c>
-      <c r="C3">
-        <v>0.79</v>
-      </c>
-      <c r="D3">
-        <v>0.72</v>
-      </c>
-      <c r="E3">
-        <v>0.75</v>
-      </c>
-      <c r="G3">
-        <v>0.82</v>
-      </c>
-      <c r="H3">
-        <v>0.93</v>
+        <v>0.96</v>
       </c>
       <c r="I3">
         <v>0.87</v>
@@ -3403,19 +2842,19 @@
         <v>0.87</v>
       </c>
       <c r="O3">
-        <v>0.74</v>
+        <v>0.78</v>
       </c>
       <c r="P3">
-        <v>0.09</v>
+        <v>0.17</v>
       </c>
       <c r="Q3">
-        <v>0.17</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="S3">
         <v>0.79</v>
       </c>
       <c r="T3">
-        <v>0.79</v>
+        <v>0.8</v>
       </c>
       <c r="U3">
         <v>0.79</v>
@@ -3429,40 +2868,40 @@
         <v>106</v>
       </c>
       <c r="C4">
-        <v>0.21</v>
+        <v>0.27</v>
       </c>
       <c r="D4">
-        <v>0.23</v>
+        <v>0.25</v>
       </c>
       <c r="E4">
-        <v>0.22</v>
+        <v>0.26</v>
       </c>
       <c r="G4">
         <v>0.48</v>
       </c>
       <c r="H4">
-        <v>0.27</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="I4">
-        <v>0.35</v>
+        <v>0.22</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="O4">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="P4">
-        <v>0.49</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="Q4">
-        <v>0.28000000000000003</v>
+        <v>0.21</v>
       </c>
       <c r="S4">
         <v>0.35</v>
@@ -3482,13 +2921,13 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>0.3</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D5">
         <v>0.67</v>
       </c>
       <c r="E5">
-        <v>0.41</v>
+        <v>0.6</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -3512,10 +2951,10 @@
         <v>0.02</v>
       </c>
       <c r="P5">
-        <v>0.22</v>
+        <v>0.44</v>
       </c>
       <c r="Q5">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -3535,22 +2974,22 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>0.15</v>
+        <v>0.19</v>
       </c>
       <c r="D6">
         <v>0.43</v>
       </c>
       <c r="E6">
-        <v>0.22</v>
+        <v>0.26</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6">
-        <v>0.43</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="I6">
-        <v>0.6</v>
+        <v>0.44</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -3562,13 +3001,13 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="P6">
         <v>0.86</v>
       </c>
       <c r="Q6">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="S6">
         <v>0</v>
@@ -3588,22 +3027,22 @@
         <v>10</v>
       </c>
       <c r="C7">
-        <v>0.46</v>
+        <v>0.4</v>
       </c>
       <c r="D7">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="E7">
-        <v>0.52</v>
+        <v>0.53</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="I7">
-        <v>0.75</v>
+        <v>0.89</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -3615,13 +3054,13 @@
         <v>0.46</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="S7">
         <v>0</v>
@@ -3630,289 +3069,6 @@
         <v>0</v>
       </c>
       <c r="U7">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U5"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:U5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" customWidth="1"/>
-    <col min="8" max="8" width="8" customWidth="1"/>
-    <col min="9" max="9" width="8.5" customWidth="1"/>
-    <col min="12" max="12" width="6.1640625" customWidth="1"/>
-    <col min="14" max="14" width="4.83203125" customWidth="1"/>
-    <col min="19" max="19" width="8.5" customWidth="1"/>
-    <col min="20" max="20" width="7.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="12"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="14"/>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="R2" s="9"/>
-      <c r="S2" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="U2" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="A3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="8">
-        <v>532</v>
-      </c>
-      <c r="C3">
-        <v>0.98</v>
-      </c>
-      <c r="D3">
-        <v>0.96</v>
-      </c>
-      <c r="E3">
-        <v>0.97</v>
-      </c>
-      <c r="G3">
-        <v>0.98</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>0.99</v>
-      </c>
-      <c r="K3">
-        <v>0.97</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>0.99</v>
-      </c>
-      <c r="O3">
-        <v>0.97</v>
-      </c>
-      <c r="P3">
-        <v>0.64</v>
-      </c>
-      <c r="Q3">
-        <v>0.77</v>
-      </c>
-      <c r="S3">
-        <v>0.97</v>
-      </c>
-      <c r="T3">
-        <v>0.98</v>
-      </c>
-      <c r="U3">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
-      <c r="A4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="8">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>0.33</v>
-      </c>
-      <c r="D4">
-        <v>0.5</v>
-      </c>
-      <c r="E4">
-        <v>0.4</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0.5</v>
-      </c>
-      <c r="I4">
-        <v>0.67</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>0.3</v>
-      </c>
-      <c r="M4">
-        <v>0.46</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="8">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="D5">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="E5">
-        <v>0.38</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="I5">
-        <v>0.44</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0.05</v>
-      </c>
-      <c r="P5">
-        <v>0.86</v>
-      </c>
-      <c r="Q5">
-        <v>0.1</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
         <v>0</v>
       </c>
     </row>

</xml_diff>